<commit_message>
no hidden nodes done
</commit_message>
<xml_diff>
--- a/results/RESULTS.xlsx
+++ b/results/RESULTS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maria\Documents\4th year\CI\Computational_intelligence\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0FFFB8EB-2C45-4EC2-960F-552E1F945DF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEFB071B-7D69-4CEE-930D-7B596F198814}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F6C3DE30-6FC2-46B6-87C2-3AED4A862E3F}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{F6C3DE30-6FC2-46B6-87C2-3AED4A862E3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>SELECTION</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>best</t>
+  </si>
+  <si>
+    <t>NUM HIDDEN NODES</t>
   </si>
 </sst>
 </file>
@@ -432,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE28FA4F-187B-4631-A118-67ED3E1A7FA1}">
-  <dimension ref="A2:S32"/>
+  <dimension ref="A2:V32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -451,9 +454,10 @@
     <col min="13" max="13" width="12.44140625" customWidth="1"/>
     <col min="14" max="14" width="15.6640625" customWidth="1"/>
     <col min="18" max="18" width="12.44140625" customWidth="1"/>
+    <col min="22" max="22" width="21.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -469,8 +473,11 @@
       <c r="R2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="V2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -521,8 +528,14 @@
         <f>AVERAGE(R3:R12)</f>
         <v>0.12759235079856554</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U3">
+        <v>5</v>
+      </c>
+      <c r="V3">
+        <v>0.10100105786603</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>3.1251842937616098E-2</v>
       </c>
@@ -538,8 +551,11 @@
       <c r="R4">
         <v>0.114653285234802</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="V4">
+        <v>0.117358589202783</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>0.120074774916743</v>
       </c>
@@ -555,8 +571,11 @@
       <c r="R5">
         <v>0.13043776443094901</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="V5">
+        <v>2.8107023201095899E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>0.14724271126338301</v>
       </c>
@@ -573,7 +592,7 @@
         <v>0.21883997033245201</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>9.7073156842692701E-2</v>
       </c>
@@ -590,7 +609,7 @@
         <v>0.147389360890258</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>0.19535979439946999</v>
       </c>
@@ -607,7 +626,7 @@
         <v>0.109473948283557</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>0.28910244875720797</v>
       </c>
@@ -624,7 +643,7 @@
         <v>0.12724773745568399</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>6.1770512312828298E-2</v>
       </c>
@@ -641,7 +660,7 @@
         <v>0.116406026244321</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>3.16632967800346E-2</v>
       </c>
@@ -658,7 +677,7 @@
         <v>0.147212305269384</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>0.12713833397755001</v>
       </c>
@@ -675,7 +694,7 @@
         <v>8.9504007603894195E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -726,8 +745,11 @@
         <f>AVERAGE(R13:R22)</f>
         <v>0.12499317307444394</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>0.120238399254905</v>
       </c>
@@ -744,7 +766,7 @@
         <v>0.13938493237369801</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>3.3943720090897897E-2</v>
       </c>
@@ -761,7 +783,7 @@
         <v>0.12739149858802201</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>0.12783036368176001</v>
       </c>

</xml_diff>